<commit_message>
Isolate the 2D plot execution functionalities.
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,47 +500,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>20</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>100</v>
-      </c>
-      <c r="I2" t="n">
-        <v>30</v>
-      </c>
-      <c r="J2" t="n">
-        <v>60</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>20</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>